<commit_message>
Added tau2 REML and DL estimates to the excel troubleshooting file
</commit_message>
<xml_diff>
--- a/code/effect_sizes_with_SE.xlsx
+++ b/code/effect_sizes_with_SE.xlsx
@@ -1,73 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u237972\Git\heterogeneity-replications\code\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
-  <si>
-    <t>Anch_d</t>
-  </si>
-  <si>
-    <t>Anch_d_SE</t>
-  </si>
-  <si>
-    <t>Quote_d</t>
-  </si>
-  <si>
-    <t>Quote_d_SE</t>
-  </si>
-  <si>
-    <t>Anch_r</t>
-  </si>
-  <si>
-    <t>Quote_r</t>
-  </si>
-  <si>
-    <t>Anch_trunc_SE</t>
-  </si>
-  <si>
-    <t>Quote_trunc_SE</t>
-  </si>
-  <si>
-    <t>Anch_nontrunc_SE</t>
-  </si>
-  <si>
-    <t>Quote_nontrunc_SE</t>
-  </si>
-  <si>
-    <t>Anch_n1</t>
-  </si>
-  <si>
-    <t>Anch_n2</t>
-  </si>
-  <si>
-    <t>Quote_n1</t>
-  </si>
-  <si>
-    <t>Quote_n2</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -115,14 +63,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -169,7 +109,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -201,10 +141,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -236,7 +175,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -412,84 +350,140 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N37"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:V37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="9.7109375" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Anch_d</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Anch_d_SE</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Quote_d</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Quote_d_SE</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Anch_r</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Quote_r</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Anch_trunc_SE</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Quote_trunc_SE</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Anch_nontrunc_SE</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Quote_nontrunc_SE</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Anch_n1</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Anch_n2</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Quote_n1</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Quote_n2</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Anch_d_tau2_DL</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Anch_d_tau2_REML</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>Quote_d_tau2_DL</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>Quote_d_tau2_REML</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>Anch_trunc_tau2_DL</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>Anch_trunc_tau2_REML</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>Quote_trunc_tau2_DL</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>Quote_trunc_tau2_REML</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
       <c r="A2">
         <v>1.097332153052516</v>
       </c>
       <c r="B2">
-        <v>0.26103456926790952</v>
+        <v>0.2610345692679095</v>
       </c>
       <c r="C2">
-        <v>0.21642035944704799</v>
+        <v>0.216420359447048</v>
       </c>
       <c r="D2">
-        <v>0.22111062247869459</v>
+        <v>0.2211106224786946</v>
       </c>
       <c r="E2">
-        <v>0.60934260236717208</v>
+        <v>0.6093426023671721</v>
       </c>
       <c r="F2">
         <v>0.1358644422005699</v>
@@ -498,13 +492,13 @@
         <v>0.1080974767815804</v>
       </c>
       <c r="H2">
-        <v>0.13635597465476601</v>
+        <v>0.136355974654766</v>
       </c>
       <c r="I2">
         <v>0.1080974767815804</v>
       </c>
       <c r="J2">
-        <v>0.13635597465476601</v>
+        <v>0.136355974654766</v>
       </c>
       <c r="K2">
         <v>37</v>
@@ -518,34 +512,58 @@
       <c r="N2">
         <v>48</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O2">
+        <v>0.02413190857629672</v>
+      </c>
+      <c r="P2">
+        <v>0.02300696206474691</v>
+      </c>
+      <c r="Q2">
+        <v>0.02309866459521323</v>
+      </c>
+      <c r="R2">
+        <v>0.02683769122440325</v>
+      </c>
+      <c r="S2">
+        <v>0.00821846143256463</v>
+      </c>
+      <c r="T2">
+        <v>0.007616870063325398</v>
+      </c>
+      <c r="U2">
+        <v>0.009865136932458201</v>
+      </c>
+      <c r="V2">
+        <v>0.01211763263342428</v>
+      </c>
+    </row>
+    <row r="3">
       <c r="A3">
         <v>1.20487961481093</v>
       </c>
       <c r="B3">
-        <v>0.25793901782832129</v>
+        <v>0.2579390178283213</v>
       </c>
       <c r="C3">
         <v>0.1896069663103345</v>
       </c>
       <c r="D3">
-        <v>0.19121914778304561</v>
+        <v>0.1912191477830456</v>
       </c>
       <c r="E3">
-        <v>0.65167343731830651</v>
+        <v>0.6516734373183065</v>
       </c>
       <c r="F3">
         <v>0.1173096483067325</v>
       </c>
       <c r="G3">
-        <v>9.9023324718332875E-2</v>
+        <v>0.09902332471833288</v>
       </c>
       <c r="H3">
         <v>0.1167892660702322</v>
       </c>
       <c r="I3">
-        <v>9.9023324718332875E-2</v>
+        <v>0.09902332471833288</v>
       </c>
       <c r="J3">
         <v>0.1167892660702322</v>
@@ -562,37 +580,61 @@
       <c r="N3">
         <v>43</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O3">
+        <v>0.02413190857629672</v>
+      </c>
+      <c r="P3">
+        <v>0.02300696206474691</v>
+      </c>
+      <c r="Q3">
+        <v>0.02309866459521323</v>
+      </c>
+      <c r="R3">
+        <v>0.02683769122440325</v>
+      </c>
+      <c r="S3">
+        <v>0.00821846143256463</v>
+      </c>
+      <c r="T3">
+        <v>0.007616870063325398</v>
+      </c>
+      <c r="U3">
+        <v>0.009865136932458201</v>
+      </c>
+      <c r="V3">
+        <v>0.01211763263342428</v>
+      </c>
+    </row>
+    <row r="4">
       <c r="A4">
         <v>0.9394934517286353</v>
       </c>
       <c r="B4">
-        <v>0.25769818303665082</v>
+        <v>0.2576981830366508</v>
       </c>
       <c r="C4">
-        <v>0.28541078995621988</v>
+        <v>0.2854107899562199</v>
       </c>
       <c r="D4">
         <v>0.2198820701244121</v>
       </c>
       <c r="E4">
-        <v>0.53938133463339666</v>
+        <v>0.5393813346333967</v>
       </c>
       <c r="F4">
-        <v>0.17897639246230709</v>
+        <v>0.1789763924623071</v>
       </c>
       <c r="G4">
         <v>0.1185494238707611</v>
       </c>
       <c r="H4">
-        <v>0.13425411215640001</v>
+        <v>0.1342541121564</v>
       </c>
       <c r="I4">
         <v>0.1185494238707611</v>
       </c>
       <c r="J4">
-        <v>0.13425411215640001</v>
+        <v>0.1342541121564</v>
       </c>
       <c r="K4">
         <v>32</v>
@@ -606,37 +648,61 @@
       <c r="N4">
         <v>45</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O4">
+        <v>0.02413190857629672</v>
+      </c>
+      <c r="P4">
+        <v>0.02300696206474691</v>
+      </c>
+      <c r="Q4">
+        <v>0.02309866459521323</v>
+      </c>
+      <c r="R4">
+        <v>0.02683769122440325</v>
+      </c>
+      <c r="S4">
+        <v>0.00821846143256463</v>
+      </c>
+      <c r="T4">
+        <v>0.007616870063325398</v>
+      </c>
+      <c r="U4">
+        <v>0.009865136932458201</v>
+      </c>
+      <c r="V4">
+        <v>0.01211763263342428</v>
+      </c>
+    </row>
+    <row r="5">
       <c r="A5">
         <v>1.935895315615427</v>
       </c>
       <c r="B5">
-        <v>0.27122493610435328</v>
+        <v>0.2712249361043533</v>
       </c>
       <c r="C5">
         <v>0.1428146276845785</v>
       </c>
       <c r="D5">
-        <v>0.20659369115471091</v>
+        <v>0.2065936911547109</v>
       </c>
       <c r="E5">
-        <v>0.87819334148003125</v>
+        <v>0.8781933414800313</v>
       </c>
       <c r="F5">
-        <v>9.0219951657641462E-2</v>
+        <v>0.09021995165764146</v>
       </c>
       <c r="G5">
-        <v>5.5120830339509673E-2</v>
+        <v>0.05512083033950967</v>
       </c>
       <c r="H5">
-        <v>0.12913537683492629</v>
+        <v>0.1291353768349263</v>
       </c>
       <c r="I5">
-        <v>5.5120830339509673E-2</v>
+        <v>0.05512083033950967</v>
       </c>
       <c r="J5">
-        <v>0.12913537683492629</v>
+        <v>0.1291353768349263</v>
       </c>
       <c r="K5">
         <v>49</v>
@@ -650,34 +716,58 @@
       <c r="N5">
         <v>48</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O5">
+        <v>0.02413190857629672</v>
+      </c>
+      <c r="P5">
+        <v>0.02300696206474691</v>
+      </c>
+      <c r="Q5">
+        <v>0.02309866459521323</v>
+      </c>
+      <c r="R5">
+        <v>0.02683769122440325</v>
+      </c>
+      <c r="S5">
+        <v>0.00821846143256463</v>
+      </c>
+      <c r="T5">
+        <v>0.007616870063325398</v>
+      </c>
+      <c r="U5">
+        <v>0.009865136932458201</v>
+      </c>
+      <c r="V5">
+        <v>0.01211763263342428</v>
+      </c>
+    </row>
+    <row r="6">
       <c r="A6">
-        <v>1.4475342760798111</v>
+        <v>1.447534276079811</v>
       </c>
       <c r="B6">
         <v>0.2430417657585584</v>
       </c>
       <c r="C6">
-        <v>0.78500610978094709</v>
+        <v>0.7850061097809471</v>
       </c>
       <c r="D6">
-        <v>0.21188278405453961</v>
+        <v>0.2118827840545396</v>
       </c>
       <c r="E6">
-        <v>0.73975604275269213</v>
+        <v>0.7397560427526921</v>
       </c>
       <c r="F6">
-        <v>0.46208003057289271</v>
+        <v>0.4620800305728927</v>
       </c>
       <c r="G6">
-        <v>7.7013109374847441E-2</v>
+        <v>0.07701310937484744</v>
       </c>
       <c r="H6">
         <v>0.1066967704979128</v>
       </c>
       <c r="I6">
-        <v>7.7013109374847441E-2</v>
+        <v>0.07701310937484744</v>
       </c>
       <c r="J6">
         <v>0.1066967704979128</v>
@@ -694,13 +784,37 @@
       <c r="N6">
         <v>49</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O6">
+        <v>0.02413190857629672</v>
+      </c>
+      <c r="P6">
+        <v>0.02300696206474691</v>
+      </c>
+      <c r="Q6">
+        <v>0.02309866459521323</v>
+      </c>
+      <c r="R6">
+        <v>0.02683769122440325</v>
+      </c>
+      <c r="S6">
+        <v>0.00821846143256463</v>
+      </c>
+      <c r="T6">
+        <v>0.007616870063325398</v>
+      </c>
+      <c r="U6">
+        <v>0.009865136932458201</v>
+      </c>
+      <c r="V6">
+        <v>0.01211763263342428</v>
+      </c>
+    </row>
+    <row r="7">
       <c r="A7">
         <v>1.909192065800019</v>
       </c>
       <c r="B7">
-        <v>0.28792769857816708</v>
+        <v>0.2879276985781671</v>
       </c>
       <c r="C7">
         <v>0.1904344975691146</v>
@@ -709,22 +823,22 @@
         <v>0.2009545659193242</v>
       </c>
       <c r="E7">
-        <v>0.87288385297103499</v>
+        <v>0.872883852971035</v>
       </c>
       <c r="F7">
         <v>0.1193462478578232</v>
       </c>
       <c r="G7">
-        <v>6.028849445657878E-2</v>
+        <v>0.06028849445657878</v>
       </c>
       <c r="H7">
-        <v>0.12418346251855571</v>
+        <v>0.1241834625185557</v>
       </c>
       <c r="I7">
-        <v>6.028849445657878E-2</v>
+        <v>0.06028849445657878</v>
       </c>
       <c r="J7">
-        <v>0.12418346251855571</v>
+        <v>0.1241834625185557</v>
       </c>
       <c r="K7">
         <v>28</v>
@@ -738,37 +852,61 @@
       <c r="N7">
         <v>43</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O7">
+        <v>0.02413190857629672</v>
+      </c>
+      <c r="P7">
+        <v>0.02300696206474691</v>
+      </c>
+      <c r="Q7">
+        <v>0.02309866459521323</v>
+      </c>
+      <c r="R7">
+        <v>0.02683769122440325</v>
+      </c>
+      <c r="S7">
+        <v>0.00821846143256463</v>
+      </c>
+      <c r="T7">
+        <v>0.007616870063325398</v>
+      </c>
+      <c r="U7">
+        <v>0.009865136932458201</v>
+      </c>
+      <c r="V7">
+        <v>0.01211763263342428</v>
+      </c>
+    </row>
+    <row r="8">
       <c r="A8">
-        <v>1.1484093423146089</v>
+        <v>1.148409342314609</v>
       </c>
       <c r="B8">
-        <v>0.25637165533473988</v>
+        <v>0.2563716553347399</v>
       </c>
       <c r="C8">
-        <v>0.53763817241420997</v>
+        <v>0.53763817241421</v>
       </c>
       <c r="D8">
-        <v>0.21990704121945751</v>
+        <v>0.2199070412194575</v>
       </c>
       <c r="E8">
-        <v>0.63070936647262277</v>
+        <v>0.6307093664726228</v>
       </c>
       <c r="F8">
-        <v>0.32580417938463407</v>
+        <v>0.3258041793846341</v>
       </c>
       <c r="G8">
         <v>0.1023306032282667</v>
       </c>
       <c r="H8">
-        <v>0.12353985221095851</v>
+        <v>0.1235398522109585</v>
       </c>
       <c r="I8">
         <v>0.1023306032282667</v>
       </c>
       <c r="J8">
-        <v>0.12353985221095851</v>
+        <v>0.1235398522109585</v>
       </c>
       <c r="K8">
         <v>34</v>
@@ -782,37 +920,61 @@
       <c r="N8">
         <v>35</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O8">
+        <v>0.02413190857629672</v>
+      </c>
+      <c r="P8">
+        <v>0.02300696206474691</v>
+      </c>
+      <c r="Q8">
+        <v>0.02309866459521323</v>
+      </c>
+      <c r="R8">
+        <v>0.02683769122440325</v>
+      </c>
+      <c r="S8">
+        <v>0.00821846143256463</v>
+      </c>
+      <c r="T8">
+        <v>0.007616870063325398</v>
+      </c>
+      <c r="U8">
+        <v>0.009865136932458201</v>
+      </c>
+      <c r="V8">
+        <v>0.01211763263342428</v>
+      </c>
+    </row>
+    <row r="9">
       <c r="A9">
-        <v>1.0148380966043651</v>
+        <v>1.014838096604365</v>
       </c>
       <c r="B9">
         <v>0.1827470959829495</v>
       </c>
       <c r="C9">
-        <v>0.68366828285780934</v>
+        <v>0.6836682828578093</v>
       </c>
       <c r="D9">
-        <v>0.15646535715651419</v>
+        <v>0.1564653571565142</v>
       </c>
       <c r="E9">
-        <v>0.56366822238357883</v>
+        <v>0.5636682223835788</v>
       </c>
       <c r="F9">
-        <v>0.40706888005056591</v>
+        <v>0.4070688800505659</v>
       </c>
       <c r="G9">
-        <v>8.0227755967434963E-2</v>
+        <v>0.08022775596743496</v>
       </c>
       <c r="H9">
-        <v>8.2866250594263044E-2</v>
+        <v>0.08286625059426304</v>
       </c>
       <c r="I9">
-        <v>8.0227755967434963E-2</v>
+        <v>0.08022775596743496</v>
       </c>
       <c r="J9">
-        <v>8.2866250594263044E-2</v>
+        <v>0.08286625059426304</v>
       </c>
       <c r="K9">
         <v>97</v>
@@ -826,25 +988,49 @@
       <c r="N9">
         <v>80</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O9">
+        <v>0.02413190857629672</v>
+      </c>
+      <c r="P9">
+        <v>0.02300696206474691</v>
+      </c>
+      <c r="Q9">
+        <v>0.02309866459521323</v>
+      </c>
+      <c r="R9">
+        <v>0.02683769122440325</v>
+      </c>
+      <c r="S9">
+        <v>0.00821846143256463</v>
+      </c>
+      <c r="T9">
+        <v>0.007616870063325398</v>
+      </c>
+      <c r="U9">
+        <v>0.009865136932458201</v>
+      </c>
+      <c r="V9">
+        <v>0.01211763263342428</v>
+      </c>
+    </row>
+    <row r="10">
       <c r="A10">
-        <v>1.1121590758947559</v>
+        <v>1.112159075894756</v>
       </c>
       <c r="B10">
-        <v>0.26453071383362342</v>
+        <v>0.2645307138336234</v>
       </c>
       <c r="C10">
-        <v>-8.8620526195886937E-2</v>
+        <v>-0.08862052619588694</v>
       </c>
       <c r="D10">
-        <v>0.18842086267987851</v>
+        <v>0.1884208626798785</v>
       </c>
       <c r="E10">
-        <v>0.61627552761175886</v>
+        <v>0.6162755276117589</v>
       </c>
       <c r="F10">
-        <v>-5.5953419165055619E-2</v>
+        <v>-0.05595341916505562</v>
       </c>
       <c r="G10">
         <v>0.1083466491215435</v>
@@ -870,37 +1056,61 @@
       <c r="N10">
         <v>54</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O10">
+        <v>0.02413190857629672</v>
+      </c>
+      <c r="P10">
+        <v>0.02300696206474691</v>
+      </c>
+      <c r="Q10">
+        <v>0.02309866459521323</v>
+      </c>
+      <c r="R10">
+        <v>0.02683769122440325</v>
+      </c>
+      <c r="S10">
+        <v>0.00821846143256463</v>
+      </c>
+      <c r="T10">
+        <v>0.007616870063325398</v>
+      </c>
+      <c r="U10">
+        <v>0.009865136932458201</v>
+      </c>
+      <c r="V10">
+        <v>0.01211763263342428</v>
+      </c>
+    </row>
+    <row r="11">
       <c r="A11">
-        <v>1.9190912658023529</v>
+        <v>1.919091265802353</v>
       </c>
       <c r="B11">
-        <v>0.29638618885842782</v>
+        <v>0.2963861888584278</v>
       </c>
       <c r="C11">
-        <v>0.28483413589202822</v>
+        <v>0.2848341358920282</v>
       </c>
       <c r="D11">
-        <v>0.19005811609585399</v>
+        <v>0.190058116095854</v>
       </c>
       <c r="E11">
-        <v>0.87484116378723753</v>
+        <v>0.8748411637872375</v>
       </c>
       <c r="F11">
-        <v>0.17823073334648901</v>
+        <v>0.178230733346489</v>
       </c>
       <c r="G11">
-        <v>6.0548942279661039E-2</v>
+        <v>0.06054894227966104</v>
       </c>
       <c r="H11">
-        <v>0.11598754341015489</v>
+        <v>0.1159875434101549</v>
       </c>
       <c r="I11">
-        <v>6.0548942279661039E-2</v>
+        <v>0.06054894227966104</v>
       </c>
       <c r="J11">
-        <v>0.11598754341015489</v>
+        <v>0.1159875434101549</v>
       </c>
       <c r="K11">
         <v>37</v>
@@ -914,37 +1124,61 @@
       <c r="N11">
         <v>54</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O11">
+        <v>0.02413190857629672</v>
+      </c>
+      <c r="P11">
+        <v>0.02300696206474691</v>
+      </c>
+      <c r="Q11">
+        <v>0.02309866459521323</v>
+      </c>
+      <c r="R11">
+        <v>0.02683769122440325</v>
+      </c>
+      <c r="S11">
+        <v>0.00821846143256463</v>
+      </c>
+      <c r="T11">
+        <v>0.007616870063325398</v>
+      </c>
+      <c r="U11">
+        <v>0.009865136932458201</v>
+      </c>
+      <c r="V11">
+        <v>0.01211763263342428</v>
+      </c>
+    </row>
+    <row r="12">
       <c r="A12">
-        <v>1.3585771617467881</v>
+        <v>1.358577161746788</v>
       </c>
       <c r="B12">
-        <v>0.14628160319411809</v>
+        <v>0.1462816031941181</v>
       </c>
       <c r="C12">
-        <v>0.37775430207192418</v>
+        <v>0.3777543020719242</v>
       </c>
       <c r="D12">
         <v>0.1212423416042427</v>
       </c>
       <c r="E12">
-        <v>0.70570284446518194</v>
+        <v>0.7057028444651819</v>
       </c>
       <c r="F12">
-        <v>0.23341932060872289</v>
+        <v>0.2334193206087229</v>
       </c>
       <c r="G12">
-        <v>4.9955547892894712E-2</v>
+        <v>0.04995554789289471</v>
       </c>
       <c r="H12">
-        <v>7.216358519118099E-2</v>
+        <v>0.07216358519118099</v>
       </c>
       <c r="I12">
-        <v>4.9955547892894712E-2</v>
+        <v>0.04995554789289471</v>
       </c>
       <c r="J12">
-        <v>7.216358519118099E-2</v>
+        <v>0.07216358519118099</v>
       </c>
       <c r="K12">
         <v>131</v>
@@ -958,37 +1192,61 @@
       <c r="N12">
         <v>140</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O12">
+        <v>0.02413190857629672</v>
+      </c>
+      <c r="P12">
+        <v>0.02300696206474691</v>
+      </c>
+      <c r="Q12">
+        <v>0.02309866459521323</v>
+      </c>
+      <c r="R12">
+        <v>0.02683769122440325</v>
+      </c>
+      <c r="S12">
+        <v>0.00821846143256463</v>
+      </c>
+      <c r="T12">
+        <v>0.007616870063325398</v>
+      </c>
+      <c r="U12">
+        <v>0.009865136932458201</v>
+      </c>
+      <c r="V12">
+        <v>0.01211763263342428</v>
+      </c>
+    </row>
+    <row r="13">
       <c r="A13">
         <v>1.299218390035781</v>
       </c>
       <c r="B13">
-        <v>0.19686015805924029</v>
+        <v>0.1968601580592403</v>
       </c>
       <c r="C13">
         <v>0.4074653025995536</v>
       </c>
       <c r="D13">
-        <v>0.16729145024061831</v>
+        <v>0.1672914502406183</v>
       </c>
       <c r="E13">
-        <v>0.68662382225876917</v>
+        <v>0.6866238222587692</v>
       </c>
       <c r="F13">
         <v>0.2518263121019903</v>
       </c>
       <c r="G13">
-        <v>7.0215324005652918E-2</v>
+        <v>0.07021532400565292</v>
       </c>
       <c r="H13">
-        <v>9.8837929567375943E-2</v>
+        <v>0.09883792956737594</v>
       </c>
       <c r="I13">
-        <v>7.0215324005652918E-2</v>
+        <v>0.07021532400565292</v>
       </c>
       <c r="J13">
-        <v>9.8837929567375943E-2</v>
+        <v>0.09883792956737594</v>
       </c>
       <c r="K13">
         <v>63</v>
@@ -1002,37 +1260,61 @@
       <c r="N13">
         <v>75</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O13">
+        <v>0.02413190857629672</v>
+      </c>
+      <c r="P13">
+        <v>0.02300696206474691</v>
+      </c>
+      <c r="Q13">
+        <v>0.02309866459521323</v>
+      </c>
+      <c r="R13">
+        <v>0.02683769122440325</v>
+      </c>
+      <c r="S13">
+        <v>0.00821846143256463</v>
+      </c>
+      <c r="T13">
+        <v>0.007616870063325398</v>
+      </c>
+      <c r="U13">
+        <v>0.009865136932458201</v>
+      </c>
+      <c r="V13">
+        <v>0.01211763263342428</v>
+      </c>
+    </row>
+    <row r="14">
       <c r="A14">
-        <v>1.2837530316649539</v>
+        <v>1.283753031664954</v>
       </c>
       <c r="B14">
         <v>0.2417971342748933</v>
       </c>
       <c r="C14">
-        <v>9.1906798844909515E-2</v>
+        <v>0.09190679884490952</v>
       </c>
       <c r="D14">
-        <v>0.20217920159145811</v>
+        <v>0.2021792015914581</v>
       </c>
       <c r="E14">
-        <v>0.68253515477122095</v>
+        <v>0.682535154771221</v>
       </c>
       <c r="F14">
-        <v>5.8123100348013122E-2</v>
+        <v>0.05812310034801312</v>
       </c>
       <c r="G14">
-        <v>8.7242780523415012E-2</v>
+        <v>0.08724278052341501</v>
       </c>
       <c r="H14">
-        <v>0.12692688720945491</v>
+        <v>0.1269268872094549</v>
       </c>
       <c r="I14">
-        <v>8.7242780523415012E-2</v>
+        <v>0.08724278052341501</v>
       </c>
       <c r="J14">
-        <v>0.12692688720945491</v>
+        <v>0.1269268872094549</v>
       </c>
       <c r="K14">
         <v>45</v>
@@ -1046,37 +1328,61 @@
       <c r="N14">
         <v>48</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O14">
+        <v>0.02413190857629672</v>
+      </c>
+      <c r="P14">
+        <v>0.02300696206474691</v>
+      </c>
+      <c r="Q14">
+        <v>0.02309866459521323</v>
+      </c>
+      <c r="R14">
+        <v>0.02683769122440325</v>
+      </c>
+      <c r="S14">
+        <v>0.00821846143256463</v>
+      </c>
+      <c r="T14">
+        <v>0.007616870063325398</v>
+      </c>
+      <c r="U14">
+        <v>0.009865136932458201</v>
+      </c>
+      <c r="V14">
+        <v>0.01211763263342428</v>
+      </c>
+    </row>
+    <row r="15">
       <c r="A15">
-        <v>1.5425613494227839</v>
+        <v>1.542561349422784</v>
       </c>
       <c r="B15">
         <v>0.3428293401733849</v>
       </c>
       <c r="C15">
-        <v>-2.8192376713551778E-2</v>
+        <v>-0.02819237671355178</v>
       </c>
       <c r="D15">
-        <v>0.21847655192217089</v>
+        <v>0.2184765519221709</v>
       </c>
       <c r="E15">
-        <v>0.77587849144581322</v>
+        <v>0.7758784914458132</v>
       </c>
       <c r="F15">
-        <v>-1.787058283758617E-2</v>
+        <v>-0.01787058283758617</v>
       </c>
       <c r="G15">
-        <v>9.9518819714592796E-2</v>
+        <v>0.0995188197145928</v>
       </c>
       <c r="H15">
-        <v>0.13762321727963131</v>
+        <v>0.1376232172796313</v>
       </c>
       <c r="I15">
-        <v>9.9518819714592796E-2</v>
+        <v>0.0995188197145928</v>
       </c>
       <c r="J15">
-        <v>0.13762321727963131</v>
+        <v>0.1376232172796313</v>
       </c>
       <c r="K15">
         <v>19</v>
@@ -1090,37 +1396,61 @@
       <c r="N15">
         <v>40</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O15">
+        <v>0.02413190857629672</v>
+      </c>
+      <c r="P15">
+        <v>0.02300696206474691</v>
+      </c>
+      <c r="Q15">
+        <v>0.02309866459521323</v>
+      </c>
+      <c r="R15">
+        <v>0.02683769122440325</v>
+      </c>
+      <c r="S15">
+        <v>0.00821846143256463</v>
+      </c>
+      <c r="T15">
+        <v>0.007616870063325398</v>
+      </c>
+      <c r="U15">
+        <v>0.009865136932458201</v>
+      </c>
+      <c r="V15">
+        <v>0.01211763263342428</v>
+      </c>
+    </row>
+    <row r="16">
       <c r="A16">
         <v>1.072291552971141</v>
       </c>
       <c r="B16">
-        <v>7.0300316685555697E-2</v>
+        <v>0.0703003166855557</v>
       </c>
       <c r="C16">
-        <v>0.44342751602585379</v>
+        <v>0.4434275160258538</v>
       </c>
       <c r="D16">
-        <v>6.4069692396068856E-2</v>
+        <v>0.06406969239606886</v>
       </c>
       <c r="E16">
-        <v>0.59268641942547651</v>
+        <v>0.5926864194254765</v>
       </c>
       <c r="F16">
-        <v>0.27151579596357273</v>
+        <v>0.2715157959635727</v>
       </c>
       <c r="G16">
-        <v>2.9663237150307269E-2</v>
+        <v>0.02966323715030727</v>
       </c>
       <c r="H16">
-        <v>3.7346467718825403E-2</v>
+        <v>0.0373464677188254</v>
       </c>
       <c r="I16">
-        <v>2.9663237150307269E-2</v>
+        <v>0.02966323715030727</v>
       </c>
       <c r="J16">
-        <v>3.7346467718825403E-2</v>
+        <v>0.0373464677188254</v>
       </c>
       <c r="K16">
         <v>472</v>
@@ -1134,34 +1464,58 @@
       <c r="N16">
         <v>487</v>
       </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O16">
+        <v>0.02413190857629672</v>
+      </c>
+      <c r="P16">
+        <v>0.02300696206474691</v>
+      </c>
+      <c r="Q16">
+        <v>0.02309866459521323</v>
+      </c>
+      <c r="R16">
+        <v>0.02683769122440325</v>
+      </c>
+      <c r="S16">
+        <v>0.00821846143256463</v>
+      </c>
+      <c r="T16">
+        <v>0.007616870063325398</v>
+      </c>
+      <c r="U16">
+        <v>0.009865136932458201</v>
+      </c>
+      <c r="V16">
+        <v>0.01211763263342428</v>
+      </c>
+    </row>
+    <row r="17">
       <c r="A17">
-        <v>1.5380017632563421</v>
+        <v>1.538001763256342</v>
       </c>
       <c r="B17">
-        <v>0.23773868134761139</v>
+        <v>0.2377386813476114</v>
       </c>
       <c r="C17">
-        <v>0.26503755581433269</v>
+        <v>0.2650375558143327</v>
       </c>
       <c r="D17">
-        <v>0.19427000447019421</v>
+        <v>0.1942700044701942</v>
       </c>
       <c r="E17">
-        <v>0.76920164807531966</v>
+        <v>0.7692016480753197</v>
       </c>
       <c r="F17">
         <v>0.16615471408672</v>
       </c>
       <c r="G17">
-        <v>6.9518994155347971E-2</v>
+        <v>0.06951899415534797</v>
       </c>
       <c r="H17">
         <v>0.1190784895230745</v>
       </c>
       <c r="I17">
-        <v>6.9518994155347971E-2</v>
+        <v>0.06951899415534797</v>
       </c>
       <c r="J17">
         <v>0.1190784895230745</v>
@@ -1178,10 +1532,34 @@
       <c r="N17">
         <v>55</v>
       </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O17">
+        <v>0.02413190857629672</v>
+      </c>
+      <c r="P17">
+        <v>0.02300696206474691</v>
+      </c>
+      <c r="Q17">
+        <v>0.02309866459521323</v>
+      </c>
+      <c r="R17">
+        <v>0.02683769122440325</v>
+      </c>
+      <c r="S17">
+        <v>0.00821846143256463</v>
+      </c>
+      <c r="T17">
+        <v>0.007616870063325398</v>
+      </c>
+      <c r="U17">
+        <v>0.009865136932458201</v>
+      </c>
+      <c r="V17">
+        <v>0.01211763263342428</v>
+      </c>
+    </row>
+    <row r="18">
       <c r="A18">
-        <v>0.98181464669786023</v>
+        <v>0.9818146466978602</v>
       </c>
       <c r="B18">
         <v>0.2000054627551815</v>
@@ -1190,22 +1568,22 @@
         <v>0.172263908148307</v>
       </c>
       <c r="D18">
-        <v>0.18143130154148321</v>
+        <v>0.1814313015414832</v>
       </c>
       <c r="E18">
-        <v>0.55566580722528236</v>
+        <v>0.5556658072252824</v>
       </c>
       <c r="F18">
         <v>0.1084319482681308</v>
       </c>
       <c r="G18">
-        <v>8.9573997316119883E-2</v>
+        <v>0.08957399731611988</v>
       </c>
       <c r="H18">
         <v>0.1128775269577646</v>
       </c>
       <c r="I18">
-        <v>8.9573997316119883E-2</v>
+        <v>0.08957399731611988</v>
       </c>
       <c r="J18">
         <v>0.1128775269577646</v>
@@ -1222,37 +1600,61 @@
       <c r="N18">
         <v>60</v>
       </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O18">
+        <v>0.02413190857629672</v>
+      </c>
+      <c r="P18">
+        <v>0.02300696206474691</v>
+      </c>
+      <c r="Q18">
+        <v>0.02309866459521323</v>
+      </c>
+      <c r="R18">
+        <v>0.02683769122440325</v>
+      </c>
+      <c r="S18">
+        <v>0.00821846143256463</v>
+      </c>
+      <c r="T18">
+        <v>0.007616870063325398</v>
+      </c>
+      <c r="U18">
+        <v>0.009865136932458201</v>
+      </c>
+      <c r="V18">
+        <v>0.01211763263342428</v>
+      </c>
+    </row>
+    <row r="19">
       <c r="A19">
         <v>1.034402183305803</v>
       </c>
       <c r="B19">
-        <v>6.160800378258148E-2</v>
+        <v>0.06160800378258148</v>
       </c>
       <c r="C19">
-        <v>0.26623875522181423</v>
+        <v>0.2662387552218142</v>
       </c>
       <c r="D19">
-        <v>5.5258711350729919E-2</v>
+        <v>0.05525871135072992</v>
       </c>
       <c r="E19">
-        <v>0.57607578449995256</v>
+        <v>0.5760757844999526</v>
       </c>
       <c r="F19">
-        <v>0.16549331616699059</v>
+        <v>0.1654933161669906</v>
       </c>
       <c r="G19">
-        <v>2.6667167814007409E-2</v>
+        <v>0.02666716781400741</v>
       </c>
       <c r="H19">
-        <v>3.3732975662370518E-2</v>
+        <v>0.03373297566237052</v>
       </c>
       <c r="I19">
-        <v>2.6667167814007409E-2</v>
+        <v>0.02666716781400741</v>
       </c>
       <c r="J19">
-        <v>3.3732975662370518E-2</v>
+        <v>0.03373297566237052</v>
       </c>
       <c r="K19">
         <v>618</v>
@@ -1266,34 +1668,58 @@
       <c r="N19">
         <v>649</v>
       </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O19">
+        <v>0.02413190857629672</v>
+      </c>
+      <c r="P19">
+        <v>0.02300696206474691</v>
+      </c>
+      <c r="Q19">
+        <v>0.02309866459521323</v>
+      </c>
+      <c r="R19">
+        <v>0.02683769122440325</v>
+      </c>
+      <c r="S19">
+        <v>0.00821846143256463</v>
+      </c>
+      <c r="T19">
+        <v>0.007616870063325398</v>
+      </c>
+      <c r="U19">
+        <v>0.009865136932458201</v>
+      </c>
+      <c r="V19">
+        <v>0.01211763263342428</v>
+      </c>
+    </row>
+    <row r="20">
       <c r="A20">
-        <v>1.7595741455240761</v>
+        <v>1.759574145524076</v>
       </c>
       <c r="B20">
-        <v>0.26340444544169062</v>
+        <v>0.2634044454416906</v>
       </c>
       <c r="C20">
-        <v>0.42430195259256592</v>
+        <v>0.4243019525925659</v>
       </c>
       <c r="D20">
         <v>0.207592946209019</v>
       </c>
       <c r="E20">
-        <v>0.83376041875464335</v>
+        <v>0.8337604187546434</v>
       </c>
       <c r="F20">
         <v>0.2627126527068751</v>
       </c>
       <c r="G20">
-        <v>6.2822811092074396E-2</v>
+        <v>0.0628228110920744</v>
       </c>
       <c r="H20">
         <v>0.1221876432541526</v>
       </c>
       <c r="I20">
-        <v>6.2822811092074396E-2</v>
+        <v>0.0628228110920744</v>
       </c>
       <c r="J20">
         <v>0.1221876432541526</v>
@@ -1310,37 +1736,61 @@
       <c r="N20">
         <v>46</v>
       </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O20">
+        <v>0.02413190857629672</v>
+      </c>
+      <c r="P20">
+        <v>0.02300696206474691</v>
+      </c>
+      <c r="Q20">
+        <v>0.02309866459521323</v>
+      </c>
+      <c r="R20">
+        <v>0.02683769122440325</v>
+      </c>
+      <c r="S20">
+        <v>0.00821846143256463</v>
+      </c>
+      <c r="T20">
+        <v>0.007616870063325398</v>
+      </c>
+      <c r="U20">
+        <v>0.009865136932458201</v>
+      </c>
+      <c r="V20">
+        <v>0.01211763263342428</v>
+      </c>
+    </row>
+    <row r="21">
       <c r="A21">
         <v>0.9978796252831772</v>
       </c>
       <c r="B21">
-        <v>0.22375082237248939</v>
+        <v>0.2237508223724894</v>
       </c>
       <c r="C21">
-        <v>0.93722920209876959</v>
+        <v>0.9372292020987696</v>
       </c>
       <c r="D21">
-        <v>0.20973182949739971</v>
+        <v>0.2097318294973997</v>
       </c>
       <c r="E21">
-        <v>0.56446681444273161</v>
+        <v>0.5644668144427316</v>
       </c>
       <c r="F21">
-        <v>0.53613549306189978</v>
+        <v>0.5361354930618998</v>
       </c>
       <c r="G21">
-        <v>9.9152084786863562E-2</v>
+        <v>0.09915208478686356</v>
       </c>
       <c r="H21">
-        <v>9.66188648580633E-2</v>
+        <v>0.0966188648580633</v>
       </c>
       <c r="I21">
-        <v>9.9152084786863562E-2</v>
+        <v>0.09915208478686356</v>
       </c>
       <c r="J21">
-        <v>9.66188648580633E-2</v>
+        <v>0.0966188648580633</v>
       </c>
       <c r="K21">
         <v>47</v>
@@ -1354,8 +1804,32 @@
       <c r="N21">
         <v>49</v>
       </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O21">
+        <v>0.02413190857629672</v>
+      </c>
+      <c r="P21">
+        <v>0.02300696206474691</v>
+      </c>
+      <c r="Q21">
+        <v>0.02309866459521323</v>
+      </c>
+      <c r="R21">
+        <v>0.02683769122440325</v>
+      </c>
+      <c r="S21">
+        <v>0.00821846143256463</v>
+      </c>
+      <c r="T21">
+        <v>0.007616870063325398</v>
+      </c>
+      <c r="U21">
+        <v>0.009865136932458201</v>
+      </c>
+      <c r="V21">
+        <v>0.01211763263342428</v>
+      </c>
+    </row>
+    <row r="22">
       <c r="A22">
         <v>1.798506487784401</v>
       </c>
@@ -1363,28 +1837,28 @@
         <v>0.2750940288154301</v>
       </c>
       <c r="C22">
-        <v>0.40439380032036643</v>
+        <v>0.4043938003203664</v>
       </c>
       <c r="D22">
-        <v>0.22256099233931631</v>
+        <v>0.2225609923393163</v>
       </c>
       <c r="E22">
-        <v>0.84442841366391541</v>
+        <v>0.8444284136639154</v>
       </c>
       <c r="F22">
         <v>0.2497064337603164</v>
       </c>
       <c r="G22">
-        <v>6.3408283995205025E-2</v>
+        <v>0.06340828399520503</v>
       </c>
       <c r="H22">
-        <v>0.13118734782019301</v>
+        <v>0.131187347820193</v>
       </c>
       <c r="I22">
-        <v>6.3408283995205025E-2</v>
+        <v>0.06340828399520503</v>
       </c>
       <c r="J22">
-        <v>0.13118734782019301</v>
+        <v>0.131187347820193</v>
       </c>
       <c r="K22">
         <v>42</v>
@@ -1398,10 +1872,34 @@
       <c r="N22">
         <v>35</v>
       </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O22">
+        <v>0.02413190857629672</v>
+      </c>
+      <c r="P22">
+        <v>0.02300696206474691</v>
+      </c>
+      <c r="Q22">
+        <v>0.02309866459521323</v>
+      </c>
+      <c r="R22">
+        <v>0.02683769122440325</v>
+      </c>
+      <c r="S22">
+        <v>0.00821846143256463</v>
+      </c>
+      <c r="T22">
+        <v>0.007616870063325398</v>
+      </c>
+      <c r="U22">
+        <v>0.009865136932458201</v>
+      </c>
+      <c r="V22">
+        <v>0.01211763263342428</v>
+      </c>
+    </row>
+    <row r="23">
       <c r="A23">
-        <v>0.92020600313333245</v>
+        <v>0.9202060031333325</v>
       </c>
       <c r="B23">
         <v>0.1768926974075328</v>
@@ -1410,25 +1908,25 @@
         <v>0.4064766839336949</v>
       </c>
       <c r="D23">
-        <v>0.15879662798451569</v>
+        <v>0.1587966279845157</v>
       </c>
       <c r="E23">
-        <v>0.52660445546734469</v>
+        <v>0.5266044554673447</v>
       </c>
       <c r="F23">
-        <v>0.25108154041674757</v>
+        <v>0.2510815404167476</v>
       </c>
       <c r="G23">
-        <v>8.2344103760685169E-2</v>
+        <v>0.08234410376068517</v>
       </c>
       <c r="H23">
-        <v>9.3823784446475086E-2</v>
+        <v>0.09382378444647509</v>
       </c>
       <c r="I23">
-        <v>8.2344103760685169E-2</v>
+        <v>0.08234410376068517</v>
       </c>
       <c r="J23">
-        <v>9.3823784446475086E-2</v>
+        <v>0.09382378444647509</v>
       </c>
       <c r="K23">
         <v>76</v>
@@ -1442,37 +1940,61 @@
       <c r="N23">
         <v>83</v>
       </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O23">
+        <v>0.02413190857629672</v>
+      </c>
+      <c r="P23">
+        <v>0.02300696206474691</v>
+      </c>
+      <c r="Q23">
+        <v>0.02309866459521323</v>
+      </c>
+      <c r="R23">
+        <v>0.02683769122440325</v>
+      </c>
+      <c r="S23">
+        <v>0.00821846143256463</v>
+      </c>
+      <c r="T23">
+        <v>0.007616870063325398</v>
+      </c>
+      <c r="U23">
+        <v>0.009865136932458201</v>
+      </c>
+      <c r="V23">
+        <v>0.01211763263342428</v>
+      </c>
+    </row>
+    <row r="24">
       <c r="A24">
-        <v>1.3998276742593849</v>
+        <v>1.399827674259385</v>
       </c>
       <c r="B24">
         <v>0.3232411153299064</v>
       </c>
       <c r="C24">
-        <v>-9.7800410910191832E-3</v>
+        <v>-0.009780041091019183</v>
       </c>
       <c r="D24">
-        <v>0.22503695477794949</v>
+        <v>0.2250369547779495</v>
       </c>
       <c r="E24">
-        <v>0.72644949345778065</v>
+        <v>0.7264494934577807</v>
       </c>
       <c r="F24">
-        <v>-6.2075259591509802E-3</v>
+        <v>-0.00620752595915098</v>
       </c>
       <c r="G24">
         <v>0.1067241875756183</v>
       </c>
       <c r="H24">
-        <v>0.14191200859103259</v>
+        <v>0.1419120085910326</v>
       </c>
       <c r="I24">
         <v>0.1067241875756183</v>
       </c>
       <c r="J24">
-        <v>0.14191200859103259</v>
+        <v>0.1419120085910326</v>
       </c>
       <c r="K24">
         <v>19</v>
@@ -1486,37 +2008,61 @@
       <c r="N24">
         <v>40</v>
       </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O24">
+        <v>0.02413190857629672</v>
+      </c>
+      <c r="P24">
+        <v>0.02300696206474691</v>
+      </c>
+      <c r="Q24">
+        <v>0.02309866459521323</v>
+      </c>
+      <c r="R24">
+        <v>0.02683769122440325</v>
+      </c>
+      <c r="S24">
+        <v>0.00821846143256463</v>
+      </c>
+      <c r="T24">
+        <v>0.007616870063325398</v>
+      </c>
+      <c r="U24">
+        <v>0.009865136932458201</v>
+      </c>
+      <c r="V24">
+        <v>0.01211763263342428</v>
+      </c>
+    </row>
+    <row r="25">
       <c r="A25">
-        <v>0.81868428200409205</v>
+        <v>0.8186842820040921</v>
       </c>
       <c r="B25">
-        <v>0.19928178565068039</v>
+        <v>0.1992817856506804</v>
       </c>
       <c r="C25">
-        <v>0.31095834650826232</v>
+        <v>0.3109583465082623</v>
       </c>
       <c r="D25">
-        <v>0.15650049462535121</v>
+        <v>0.1565004946253512</v>
       </c>
       <c r="E25">
-        <v>0.47797327992672012</v>
+        <v>0.4779732799267201</v>
       </c>
       <c r="F25">
         <v>0.1932783786741166</v>
       </c>
       <c r="G25">
-        <v>9.8448185383583617E-2</v>
+        <v>0.09844818538358362</v>
       </c>
       <c r="H25">
-        <v>9.4666429050645984E-2</v>
+        <v>0.09466642905064598</v>
       </c>
       <c r="I25">
-        <v>9.8448185383583617E-2</v>
+        <v>0.09844818538358362</v>
       </c>
       <c r="J25">
-        <v>9.4666429050645984E-2</v>
+        <v>0.09466642905064598</v>
       </c>
       <c r="K25">
         <v>50</v>
@@ -1530,37 +2076,61 @@
       <c r="N25">
         <v>75</v>
       </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O25">
+        <v>0.02413190857629672</v>
+      </c>
+      <c r="P25">
+        <v>0.02300696206474691</v>
+      </c>
+      <c r="Q25">
+        <v>0.02309866459521323</v>
+      </c>
+      <c r="R25">
+        <v>0.02683769122440325</v>
+      </c>
+      <c r="S25">
+        <v>0.00821846143256463</v>
+      </c>
+      <c r="T25">
+        <v>0.007616870063325398</v>
+      </c>
+      <c r="U25">
+        <v>0.009865136932458201</v>
+      </c>
+      <c r="V25">
+        <v>0.01211763263342428</v>
+      </c>
+    </row>
+    <row r="26">
       <c r="A26">
-        <v>1.2783208935302539</v>
+        <v>1.278320893530254</v>
       </c>
       <c r="B26">
         <v>0.1719109969194382</v>
       </c>
       <c r="C26">
-        <v>0.34440350269612541</v>
+        <v>0.3444035026961254</v>
       </c>
       <c r="D26">
-        <v>0.14814439309116631</v>
+        <v>0.1481443930911663</v>
       </c>
       <c r="E26">
-        <v>0.67793204959244002</v>
+        <v>0.67793204959244</v>
       </c>
       <c r="F26">
         <v>0.2135689480782475</v>
       </c>
       <c r="G26">
-        <v>6.2361769093092233E-2</v>
+        <v>0.06236176909309223</v>
       </c>
       <c r="H26">
-        <v>8.894163890624382E-2</v>
+        <v>0.08894163890624382</v>
       </c>
       <c r="I26">
-        <v>6.2361769093092233E-2</v>
+        <v>0.06236176909309223</v>
       </c>
       <c r="J26">
-        <v>8.894163890624382E-2</v>
+        <v>0.08894163890624382</v>
       </c>
       <c r="K26">
         <v>81</v>
@@ -1574,34 +2144,58 @@
       <c r="N26">
         <v>86</v>
       </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O26">
+        <v>0.02413190857629672</v>
+      </c>
+      <c r="P26">
+        <v>0.02300696206474691</v>
+      </c>
+      <c r="Q26">
+        <v>0.02309866459521323</v>
+      </c>
+      <c r="R26">
+        <v>0.02683769122440325</v>
+      </c>
+      <c r="S26">
+        <v>0.00821846143256463</v>
+      </c>
+      <c r="T26">
+        <v>0.007616870063325398</v>
+      </c>
+      <c r="U26">
+        <v>0.009865136932458201</v>
+      </c>
+      <c r="V26">
+        <v>0.01211763263342428</v>
+      </c>
+    </row>
+    <row r="27">
       <c r="A27">
         <v>1.242446335920548</v>
       </c>
       <c r="B27">
-        <v>0.24429331786549061</v>
+        <v>0.2442933178654906</v>
       </c>
       <c r="C27">
-        <v>0.51319520598041379</v>
+        <v>0.5131952059804138</v>
       </c>
       <c r="D27">
-        <v>0.21827274478417999</v>
+        <v>0.21827274478418</v>
       </c>
       <c r="E27">
-        <v>0.66737785415524142</v>
+        <v>0.6673778541552414</v>
       </c>
       <c r="F27">
-        <v>0.31472978514430527</v>
+        <v>0.3147297851443053</v>
       </c>
       <c r="G27">
-        <v>9.0923370546364207E-2</v>
+        <v>0.09092337054636421</v>
       </c>
       <c r="H27">
         <v>0.1245946780717256</v>
       </c>
       <c r="I27">
-        <v>9.0923370546364207E-2</v>
+        <v>0.09092337054636421</v>
       </c>
       <c r="J27">
         <v>0.1245946780717256</v>
@@ -1618,8 +2212,32 @@
       <c r="N27">
         <v>41</v>
       </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O27">
+        <v>0.02413190857629672</v>
+      </c>
+      <c r="P27">
+        <v>0.02300696206474691</v>
+      </c>
+      <c r="Q27">
+        <v>0.02309866459521323</v>
+      </c>
+      <c r="R27">
+        <v>0.02683769122440325</v>
+      </c>
+      <c r="S27">
+        <v>0.00821846143256463</v>
+      </c>
+      <c r="T27">
+        <v>0.007616870063325398</v>
+      </c>
+      <c r="U27">
+        <v>0.009865136932458201</v>
+      </c>
+      <c r="V27">
+        <v>0.01211763263342428</v>
+      </c>
+    </row>
+    <row r="28">
       <c r="A28">
         <v>1.147495786262811</v>
       </c>
@@ -1627,28 +2245,28 @@
         <v>0.1587618887645279</v>
       </c>
       <c r="C28">
-        <v>0.38014583866277912</v>
+        <v>0.3801458386627791</v>
       </c>
       <c r="D28">
         <v>0.1354756076965295</v>
       </c>
       <c r="E28">
-        <v>0.62583758324151884</v>
+        <v>0.6258375832415188</v>
       </c>
       <c r="F28">
-        <v>0.23459779099685871</v>
+        <v>0.2345977909968587</v>
       </c>
       <c r="G28">
-        <v>6.3544763337144039E-2</v>
+        <v>0.06354476333714404</v>
       </c>
       <c r="H28">
-        <v>8.0475271509660912E-2</v>
+        <v>0.08047527150966091</v>
       </c>
       <c r="I28">
-        <v>6.3544763337144039E-2</v>
+        <v>0.06354476333714404</v>
       </c>
       <c r="J28">
-        <v>8.0475271509660912E-2</v>
+        <v>0.08047527150966091</v>
       </c>
       <c r="K28">
         <v>101</v>
@@ -1662,25 +2280,49 @@
       <c r="N28">
         <v>123</v>
       </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O28">
+        <v>0.02413190857629672</v>
+      </c>
+      <c r="P28">
+        <v>0.02300696206474691</v>
+      </c>
+      <c r="Q28">
+        <v>0.02309866459521323</v>
+      </c>
+      <c r="R28">
+        <v>0.02683769122440325</v>
+      </c>
+      <c r="S28">
+        <v>0.00821846143256463</v>
+      </c>
+      <c r="T28">
+        <v>0.007616870063325398</v>
+      </c>
+      <c r="U28">
+        <v>0.009865136932458201</v>
+      </c>
+      <c r="V28">
+        <v>0.01211763263342428</v>
+      </c>
+    </row>
+    <row r="29">
       <c r="A29">
         <v>0.9948256041537975</v>
       </c>
       <c r="B29">
-        <v>0.26682425001616278</v>
+        <v>0.2668242500161628</v>
       </c>
       <c r="C29">
-        <v>0.55100034305169909</v>
+        <v>0.5510003430516991</v>
       </c>
       <c r="D29">
-        <v>0.23032239090768891</v>
+        <v>0.2303223909076889</v>
       </c>
       <c r="E29">
-        <v>0.56069055743699214</v>
+        <v>0.5606905574369921</v>
       </c>
       <c r="F29">
-        <v>0.33545742714507598</v>
+        <v>0.335457427145076</v>
       </c>
       <c r="G29">
         <v>0.118546369952856</v>
@@ -1706,34 +2348,58 @@
       <c r="N29">
         <v>46</v>
       </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O29">
+        <v>0.02413190857629672</v>
+      </c>
+      <c r="P29">
+        <v>0.02300696206474691</v>
+      </c>
+      <c r="Q29">
+        <v>0.02309866459521323</v>
+      </c>
+      <c r="R29">
+        <v>0.02683769122440325</v>
+      </c>
+      <c r="S29">
+        <v>0.00821846143256463</v>
+      </c>
+      <c r="T29">
+        <v>0.007616870063325398</v>
+      </c>
+      <c r="U29">
+        <v>0.009865136932458201</v>
+      </c>
+      <c r="V29">
+        <v>0.01211763263342428</v>
+      </c>
+    </row>
+    <row r="30">
       <c r="A30">
         <v>1.396137419809403</v>
       </c>
       <c r="B30">
-        <v>0.20942635141545479</v>
+        <v>0.2094263514154548</v>
       </c>
       <c r="C30">
-        <v>0.49608365011864058</v>
+        <v>0.4960836501186406</v>
       </c>
       <c r="D30">
         <v>0.1808397815380843</v>
       </c>
       <c r="E30">
-        <v>0.72101490716840955</v>
+        <v>0.7210149071684096</v>
       </c>
       <c r="F30">
-        <v>0.30357070752227361</v>
+        <v>0.3035707075222736</v>
       </c>
       <c r="G30">
-        <v>6.9270959164279278E-2</v>
+        <v>0.06927095916427928</v>
       </c>
       <c r="H30">
         <v>0.1036845972621709</v>
       </c>
       <c r="I30">
-        <v>6.9270959164279278E-2</v>
+        <v>0.06927095916427928</v>
       </c>
       <c r="J30">
         <v>0.1036845972621709</v>
@@ -1750,10 +2416,34 @@
       <c r="N30">
         <v>58</v>
       </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O30">
+        <v>0.02413190857629672</v>
+      </c>
+      <c r="P30">
+        <v>0.02300696206474691</v>
+      </c>
+      <c r="Q30">
+        <v>0.02309866459521323</v>
+      </c>
+      <c r="R30">
+        <v>0.02683769122440325</v>
+      </c>
+      <c r="S30">
+        <v>0.00821846143256463</v>
+      </c>
+      <c r="T30">
+        <v>0.007616870063325398</v>
+      </c>
+      <c r="U30">
+        <v>0.009865136932458201</v>
+      </c>
+      <c r="V30">
+        <v>0.01211763263342428</v>
+      </c>
+    </row>
+    <row r="31">
       <c r="A31">
-        <v>1.1331580107910879</v>
+        <v>1.133158010791088</v>
       </c>
       <c r="B31">
         <v>0.2167774232364757</v>
@@ -1762,22 +2452,22 @@
         <v>-0.2623733643775496</v>
       </c>
       <c r="D31">
-        <v>0.16778382861091579</v>
+        <v>0.1677838286109158</v>
       </c>
       <c r="E31">
-        <v>0.62246118162657738</v>
+        <v>0.6224611816265774</v>
       </c>
       <c r="F31">
         <v>-0.1639824331082301</v>
       </c>
       <c r="G31">
-        <v>8.7557017905776163E-2</v>
+        <v>0.08755701790577616</v>
       </c>
       <c r="H31">
         <v>0.1027034635966156</v>
       </c>
       <c r="I31">
-        <v>8.7557017905776163E-2</v>
+        <v>0.08755701790577616</v>
       </c>
       <c r="J31">
         <v>0.1027034635966156</v>
@@ -1794,25 +2484,49 @@
       <c r="N31">
         <v>67</v>
       </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O31">
+        <v>0.02413190857629672</v>
+      </c>
+      <c r="P31">
+        <v>0.02300696206474691</v>
+      </c>
+      <c r="Q31">
+        <v>0.02309866459521323</v>
+      </c>
+      <c r="R31">
+        <v>0.02683769122440325</v>
+      </c>
+      <c r="S31">
+        <v>0.00821846143256463</v>
+      </c>
+      <c r="T31">
+        <v>0.007616870063325398</v>
+      </c>
+      <c r="U31">
+        <v>0.009865136932458201</v>
+      </c>
+      <c r="V31">
+        <v>0.01211763263342428</v>
+      </c>
+    </row>
+    <row r="32">
       <c r="A32">
-        <v>0.78093221513935274</v>
+        <v>0.7809322151393527</v>
       </c>
       <c r="B32">
-        <v>0.23661598686266111</v>
+        <v>0.2366159868626611</v>
       </c>
       <c r="C32">
-        <v>0.15716751861216791</v>
+        <v>0.1571675186121679</v>
       </c>
       <c r="D32">
-        <v>0.22271737390992111</v>
+        <v>0.2227173739099211</v>
       </c>
       <c r="E32">
         <v>0.4609806667434112</v>
       </c>
       <c r="F32">
-        <v>9.9385967777915307E-2</v>
+        <v>0.09938596777791531</v>
       </c>
       <c r="G32">
         <v>0.1194515547467216</v>
@@ -1838,34 +2552,58 @@
       <c r="N32">
         <v>39</v>
       </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O32">
+        <v>0.02413190857629672</v>
+      </c>
+      <c r="P32">
+        <v>0.02300696206474691</v>
+      </c>
+      <c r="Q32">
+        <v>0.02309866459521323</v>
+      </c>
+      <c r="R32">
+        <v>0.02683769122440325</v>
+      </c>
+      <c r="S32">
+        <v>0.00821846143256463</v>
+      </c>
+      <c r="T32">
+        <v>0.007616870063325398</v>
+      </c>
+      <c r="U32">
+        <v>0.009865136932458201</v>
+      </c>
+      <c r="V32">
+        <v>0.01211763263342428</v>
+      </c>
+    </row>
+    <row r="33">
       <c r="A33">
-        <v>1.2513117651020771</v>
+        <v>1.251311765102077</v>
       </c>
       <c r="B33">
-        <v>0.23067517460353121</v>
+        <v>0.2306751746035312</v>
       </c>
       <c r="C33">
-        <v>0.30500077817378951</v>
+        <v>0.3050007781737895</v>
       </c>
       <c r="D33">
         <v>0.1943913303149051</v>
       </c>
       <c r="E33">
-        <v>0.66935783656501568</v>
+        <v>0.6693578365650157</v>
       </c>
       <c r="F33">
         <v>0.1903468584283754</v>
       </c>
       <c r="G33">
-        <v>8.5440045835441444E-2</v>
+        <v>0.08544004583544144</v>
       </c>
       <c r="H33">
         <v>0.1179580533239641</v>
       </c>
       <c r="I33">
-        <v>8.5440045835441444E-2</v>
+        <v>0.08544004583544144</v>
       </c>
       <c r="J33">
         <v>0.1179580533239641</v>
@@ -1882,34 +2620,58 @@
       <c r="N33">
         <v>59</v>
       </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O33">
+        <v>0.02413190857629672</v>
+      </c>
+      <c r="P33">
+        <v>0.02300696206474691</v>
+      </c>
+      <c r="Q33">
+        <v>0.02309866459521323</v>
+      </c>
+      <c r="R33">
+        <v>0.02683769122440325</v>
+      </c>
+      <c r="S33">
+        <v>0.00821846143256463</v>
+      </c>
+      <c r="T33">
+        <v>0.007616870063325398</v>
+      </c>
+      <c r="U33">
+        <v>0.009865136932458201</v>
+      </c>
+      <c r="V33">
+        <v>0.01211763263342428</v>
+      </c>
+    </row>
+    <row r="34">
       <c r="A34">
-        <v>1.1579618408181691</v>
+        <v>1.157961840818169</v>
       </c>
       <c r="B34">
-        <v>0.23372453553925679</v>
+        <v>0.2337245355392568</v>
       </c>
       <c r="C34">
         <v>0.2220125663635521</v>
       </c>
       <c r="D34">
-        <v>0.20695115038287509</v>
+        <v>0.2069511503828751</v>
       </c>
       <c r="E34">
-        <v>0.63152875014053822</v>
+        <v>0.6315287501405382</v>
       </c>
       <c r="F34">
         <v>0.1390980845344299</v>
       </c>
       <c r="G34">
-        <v>9.2908668792159893E-2</v>
+        <v>0.09290866879215989</v>
       </c>
       <c r="H34">
         <v>0.1273946595526094</v>
       </c>
       <c r="I34">
-        <v>9.2908668792159893E-2</v>
+        <v>0.09290866879215989</v>
       </c>
       <c r="J34">
         <v>0.1273946595526094</v>
@@ -1926,34 +2688,58 @@
       <c r="N34">
         <v>41</v>
       </c>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O34">
+        <v>0.02413190857629672</v>
+      </c>
+      <c r="P34">
+        <v>0.02300696206474691</v>
+      </c>
+      <c r="Q34">
+        <v>0.02309866459521323</v>
+      </c>
+      <c r="R34">
+        <v>0.02683769122440325</v>
+      </c>
+      <c r="S34">
+        <v>0.00821846143256463</v>
+      </c>
+      <c r="T34">
+        <v>0.007616870063325398</v>
+      </c>
+      <c r="U34">
+        <v>0.009865136932458201</v>
+      </c>
+      <c r="V34">
+        <v>0.01211763263342428</v>
+      </c>
+    </row>
+    <row r="35">
       <c r="A35">
-        <v>1.1722829405168009</v>
+        <v>1.172282940516801</v>
       </c>
       <c r="B35">
-        <v>0.23766292554834939</v>
+        <v>0.2376629255483494</v>
       </c>
       <c r="C35">
-        <v>0.64834024226682574</v>
+        <v>0.6483402422668257</v>
       </c>
       <c r="D35">
         <v>0.2021858610667876</v>
       </c>
       <c r="E35">
-        <v>0.63869000268176612</v>
+        <v>0.6386900026817661</v>
       </c>
       <c r="F35">
-        <v>0.38992173176726619</v>
+        <v>0.3899217317672662</v>
       </c>
       <c r="G35">
-        <v>9.3355600791603835E-2</v>
+        <v>0.09335560079160384</v>
       </c>
       <c r="H35">
         <v>0.109045830011426</v>
       </c>
       <c r="I35">
-        <v>9.3355600791603835E-2</v>
+        <v>0.09335560079160384</v>
       </c>
       <c r="J35">
         <v>0.109045830011426</v>
@@ -1970,37 +2756,61 @@
       <c r="N35">
         <v>52</v>
       </c>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O35">
+        <v>0.02413190857629672</v>
+      </c>
+      <c r="P35">
+        <v>0.02300696206474691</v>
+      </c>
+      <c r="Q35">
+        <v>0.02309866459521323</v>
+      </c>
+      <c r="R35">
+        <v>0.02683769122440325</v>
+      </c>
+      <c r="S35">
+        <v>0.00821846143256463</v>
+      </c>
+      <c r="T35">
+        <v>0.007616870063325398</v>
+      </c>
+      <c r="U35">
+        <v>0.009865136932458201</v>
+      </c>
+      <c r="V35">
+        <v>0.01211763263342428</v>
+      </c>
+    </row>
+    <row r="36">
       <c r="A36">
-        <v>0.91422391415337767</v>
+        <v>0.9142239141533777</v>
       </c>
       <c r="B36">
-        <v>0.23726705631882961</v>
+        <v>0.2372670563188296</v>
       </c>
       <c r="C36">
-        <v>-0.35459104885107862</v>
+        <v>-0.3545910488510786</v>
       </c>
       <c r="D36">
-        <v>0.21246875341414989</v>
+        <v>0.2124687534141499</v>
       </c>
       <c r="E36">
-        <v>0.52412445412108699</v>
+        <v>0.524124454121087</v>
       </c>
       <c r="F36">
-        <v>-0.22119057617422949</v>
+        <v>-0.2211905761742295</v>
       </c>
       <c r="G36">
         <v>0.1108173435039157</v>
       </c>
       <c r="H36">
-        <v>0.12766496450101081</v>
+        <v>0.1276649645010108</v>
       </c>
       <c r="I36">
         <v>0.1108173435039157</v>
       </c>
       <c r="J36">
-        <v>0.12766496450101081</v>
+        <v>0.1276649645010108</v>
       </c>
       <c r="K36">
         <v>48</v>
@@ -2014,34 +2824,58 @@
       <c r="N36">
         <v>45</v>
       </c>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O36">
+        <v>0.02413190857629672</v>
+      </c>
+      <c r="P36">
+        <v>0.02300696206474691</v>
+      </c>
+      <c r="Q36">
+        <v>0.02309866459521323</v>
+      </c>
+      <c r="R36">
+        <v>0.02683769122440325</v>
+      </c>
+      <c r="S36">
+        <v>0.00821846143256463</v>
+      </c>
+      <c r="T36">
+        <v>0.007616870063325398</v>
+      </c>
+      <c r="U36">
+        <v>0.009865136932458201</v>
+      </c>
+      <c r="V36">
+        <v>0.01211763263342428</v>
+      </c>
+    </row>
+    <row r="37">
       <c r="A37">
         <v>1.167671887348648</v>
       </c>
       <c r="B37">
-        <v>0.24385657577478551</v>
+        <v>0.2438565757747855</v>
       </c>
       <c r="C37">
-        <v>0.22587364358900011</v>
+        <v>0.2258736435890001</v>
       </c>
       <c r="D37">
-        <v>0.21523233520360111</v>
+        <v>0.2152323352036011</v>
       </c>
       <c r="E37">
-        <v>0.63774779126496639</v>
+        <v>0.6377477912649664</v>
       </c>
       <c r="F37">
         <v>0.1422399655793247</v>
       </c>
       <c r="G37">
-        <v>9.6020353943297887E-2</v>
+        <v>0.09602035394329789</v>
       </c>
       <c r="H37">
         <v>0.1330125460360814</v>
       </c>
       <c r="I37">
-        <v>9.6020353943297887E-2</v>
+        <v>0.09602035394329789</v>
       </c>
       <c r="J37">
         <v>0.1330125460360814</v>
@@ -2057,6 +2891,30 @@
       </c>
       <c r="N37">
         <v>45</v>
+      </c>
+      <c r="O37">
+        <v>0.02413190857629672</v>
+      </c>
+      <c r="P37">
+        <v>0.02300696206474691</v>
+      </c>
+      <c r="Q37">
+        <v>0.02309866459521323</v>
+      </c>
+      <c r="R37">
+        <v>0.02683769122440325</v>
+      </c>
+      <c r="S37">
+        <v>0.00821846143256463</v>
+      </c>
+      <c r="T37">
+        <v>0.007616870063325398</v>
+      </c>
+      <c r="U37">
+        <v>0.009865136932458201</v>
+      </c>
+      <c r="V37">
+        <v>0.01211763263342428</v>
       </c>
     </row>
   </sheetData>

</xml_diff>